<commit_message>
Update automatico via Actualizar 05-14-2020 16-03-32
</commit_message>
<xml_diff>
--- a/datacovidgt/00 DATACOVID Trabajo_GT.xlsx
+++ b/datacovidgt/00 DATACOVID Trabajo_GT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="194" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B2754B88-E2F4-4212-81A8-AF673305AE9C}"/>
+  <xr:revisionPtr revIDLastSave="338" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2779D902-425F-48FD-9820-9BD06B169BEE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56D738C3-148A-420A-8894-4D7B344C02BA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="94">
   <si>
     <t>Fuente</t>
   </si>
@@ -74,184 +74,218 @@
     <t>División administrativa</t>
   </si>
   <si>
-    <t>Poder Judicial de Honduras</t>
+    <t>Organismo Judicial</t>
   </si>
   <si>
     <t>Trabajo</t>
   </si>
   <si>
-    <t>La potestad de impartir justicia emana del pueblo y se imparte gratuitamente en nombre del Estado, por magistrados y jueces independientes, únicamente sometidos a la Constitución y a las leyes. El Poder Judicial se integra por una Corte Suprema de Justicia, por las Cortes de Apelaciones, los Juzgados, y demás dependencias que señale la Ley</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=comunicado-del-poder-judicial</t>
-  </si>
-  <si>
-    <t>Se autoriza para que todo Servidor Judicial mayor a 60 años de edad, permanezca en su
-casa y que, dependiendo de la naturaleza de las tareas asignadas, el trabajo bajo su
-responsabilidad pueda desarrollarlo de manera remota a través de las plataformas
-informáticas disponibles o de la forma como sea indicada por su superior jerárquico.</t>
-  </si>
-  <si>
-    <t>15/3/2020</t>
+    <t>Conforme lo establece la Constitución Política de la República de Guatemala, el Organismo Judicial es el encargado de impartir justicia, con independencia y potestad de juzgar. La Ley del Organismo Judicial cita que en ejercicio de la soberanía delegada por el pueblo, imparte justicia en concordancia con el texto constitucional.</t>
+  </si>
+  <si>
+    <t>https://legal.dca.gob.gt/GestionDocumento/VisualizarDocumento?verDocumentoPrevia=True&amp;versionImpresa=False&amp;doc=59663</t>
+  </si>
+  <si>
+    <t>Se amplia suspensión de las labores de los organismos juridisccionales y administrativas del 12 al 18 de mayo de 2020, inclusive, extendiendose ésta como licencia con goce de salario para todo el personal administratvio y judicial</t>
+  </si>
+  <si>
+    <t>http://www.oj.gob.gt/</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Ministerial</t>
+  </si>
+  <si>
+    <t>Universidad de San Carlos de Guatemala</t>
+  </si>
+  <si>
+    <t>Educacion</t>
+  </si>
+  <si>
+    <t>La Universidad de San Carlos de Guatemala, es la universidad más grande de Guatemala y la única universidad pública del País.</t>
+  </si>
+  <si>
+    <t>https://www.usac.edu.gt/adminwww/actas_csu/ACTA_No._12-2020.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan de contingencia en la universidad de San Carlos de
+Guatemala por la emergencia en el País debido a la
+pandemia por el nuevo coronavirus (covid-19).
+</t>
+  </si>
+  <si>
+    <t>https://www.usac.edu.gt/</t>
+  </si>
+  <si>
+    <t>22/3/2020</t>
+  </si>
+  <si>
+    <t>Congreso Nacional de la República de Guatemala</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>El Organismo Legislativo de la República de Guatemala (OL) es uno de los organismos del Estado, que ejerce el poder legislativo. Es decir, que tiene la potestad legislativa para hacer las leyes que favorezcan al desarrollo integral del país, así como, procurar el bienestar común entre los habitantes. Está compuesto por los diputados del Congreso de la República y por el personal técnico y administrativo.</t>
+  </si>
+  <si>
+    <t>https://legal.dca.gob.gt/GestionDocumento/VisualizarDocumento?verDocumentoPrevia=True&amp;versionImpresa=False&amp;doc=59621</t>
+  </si>
+  <si>
+    <t>Ratificación de la Prórroga del Estado de Calamidad Pública, por 30 dias mas.</t>
+  </si>
+  <si>
+    <t>https://www.congreso.gob.gt/</t>
+  </si>
+  <si>
+    <t>Secretaría General de la Presidencia de la República de Guatemala</t>
+  </si>
+  <si>
+    <t>La Secretaría General de la Presidencia de la República (SGP) es el órgano responsable del apoyo jurídico y administrativo con carácter inmediato y constante del Presidente de la República. Su función es tramitar los asuntos de Gobierno del Despacho del Presidente.</t>
+  </si>
+  <si>
+    <t>https://legal.dca.gob.gt/GestionDocumento/VisualizarDocumento?verDocumentoPrevia=True&amp;versionImpresa=False&amp;doc=59265</t>
+  </si>
+  <si>
+    <t>Disposiciones Presidenciales en caso de calamidad pública</t>
+  </si>
+  <si>
+    <t>https://www.mintrabajo.gob.gt/images/Publicaciones/Coronavirus/Decreto_Gubernativo_No._5-2020.pdf</t>
+  </si>
+  <si>
+    <t>16/3/2020</t>
+  </si>
+  <si>
+    <t>Prórroga del Estado de Calamidad Pública y órdenes para el estricto cumplimiento</t>
+  </si>
+  <si>
+    <t>https://sgp.gob.gt/</t>
+  </si>
+  <si>
+    <t>20/04/2020</t>
+  </si>
+  <si>
+    <t>Superintendencia de Administracion Tributaria</t>
+  </si>
+  <si>
+    <t>Aduanas</t>
+  </si>
+  <si>
+    <t>La Superintendencia de Administración Tributaria (SAT) es una institución descentralizada del Estado de Guatemala que tiene competencia y jurisdicción en todo el país. El principal objetivo de la SAT es ejercer con exclusividad las funciones de administración tributaria contenidas en la ley orgánica. Ejerce funciones específicas como: administración del régimen tributario, administración del sistema aduanero, administración del sistema de recaudación, establecer y operar procedimientos que faciliten a los contribuyentes el cumplimiento de sus obligaciones tributarias y otras funciones más.</t>
+  </si>
+  <si>
+    <t>https://portal.sat.gob.gt/portal/noticias/medidas-administrativas-y-operativas-implementadas-para-contrarrestar-el-impacto-comercial-por-la-pandemia/</t>
+  </si>
+  <si>
+    <t>Documento para Atender la emergencia del COVID-19 por parte del Servicio Aduanero de Guatemala
+Acciones de parte del Servicio Aduanero derivadas de la declaratoria de emergencia y con ocasión a la disminución de personal de los usuarios de comercio exterior.</t>
+  </si>
+  <si>
+    <t>https://portal.sat.gob.gt/portal/</t>
+  </si>
+  <si>
+    <t>Ministerio de Trabajo y Previsión Social</t>
+  </si>
+  <si>
+    <t>El Ministerio de Trabajo y Previsión Social de la República de Guatemala (MINTRAB), es la institución estatal encargada de velar y promover el cumplimiento eficiente y eficaz de la legislación, políticas y programas relativos al trabajo y la previsión social, en beneficio de la sociedad y busca ser un Ministerio que promueva la cultura de respeto a la legislación laboral y el bienestar de la sociedad.</t>
+  </si>
+  <si>
+    <t>https://www.mintrabajo.gob.gt/images/Publicaciones/Coronavirus/Acuerdo_Ministerial_140-2020.pdf</t>
+  </si>
+  <si>
+    <t>Normativa para suspensión de contrados de trabajo por mergencia del COVID-19</t>
+  </si>
+  <si>
+    <t>https://www.mintrabajo.gob.gt/</t>
+  </si>
+  <si>
+    <t>23/3/2020</t>
+  </si>
+  <si>
+    <t>Ministerio de Economica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Ministerio de Economía (MINECO) es el ministerio del Gobierno de Guatemala encargado de hacer cumplir el régimen jurídico relativo al desarrollo de las actividades productivas no agropecuarias, del comercio interno y externo, de la protección al consumidor, del fomento a la competencia, de la represión legal de la competencia desleal, de la limitación al funcionamiento de empresas monopólicas; de inversión nacional y extranjera, de promoción a la competitividad, del desarrollo industrial y comercial. </t>
+  </si>
+  <si>
+    <t>https://www.mineco.gob.gt/</t>
+  </si>
+  <si>
+    <t>Reglamento para el Otorgamiento del Beneficio del Fondo para la Protección del Empleo</t>
+  </si>
+  <si>
+    <t>https://www.mintrabajo.gob.gt/images/Publicaciones/Coronavirus/Reglamento_Fondo_Protec_Empleo_-_Acdo_Gub_58-2020.pdf</t>
+  </si>
+  <si>
+    <t>Superintendencia de Bancos</t>
+  </si>
+  <si>
+    <t>Financiero</t>
+  </si>
+  <si>
+    <t>La Superintendencia de Bancos de Guatemala, (SIB), organizada conforme a la ley, es el órgano que ejercerá la vigilancia e inspección de bancos, instituciones de crédito, empresas financieras, entidades afianzadoras, de seguros y las demás que la ley disponga.</t>
+  </si>
+  <si>
+    <t>https://www.sib.gob.gt/</t>
+  </si>
+  <si>
+    <t>Medidas temporales especiales para atender la coyuntura
+derivada de la pandemia denominada COVID-19, que pueden ser observadas por las instituciones supervisadas por la Superintendencia de Bancos que otorgan financiamiento</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/MARN%201/Downloads/JM-32-2020%20Para%20atender%20la%20coyuntura%20derivada%20de%20la%20pandemia%20denominada%20COVID-19.pdf</t>
+  </si>
+  <si>
+    <t>19/3/2020</t>
+  </si>
+  <si>
+    <t>Comision Nacional de Bancos y Seguro (CNBS)</t>
+  </si>
+  <si>
+    <t>Institución que por mandato constitucional tiene la responsabilidad de velar por la estabilidad y solvencia del sistema financiero y demás supervisados, su regulación, supervisión y control. Asimismo, vigilamos la transparencia y que se respeten los derechos de los usuarios financieros, así como coadyuvamos con el sistema de prevención y detección del lavado activos y financiamiento al terrorismo, y contribuimos a promover la educación e inclusión financiera, a fin de salvaguardar el interés público.</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=cnbs-22-3</t>
+  </si>
+  <si>
+    <t>Las instituciones por la CNBS que realizan operaciones de crédito, podran otorgar periodos de gracia a los deudores que sean afectados por la reduccion de sus flujos de efectivo los cuales se podran otorgar hasta el 30 de junio de 2020.</t>
+  </si>
+  <si>
+    <t>21/3/2020</t>
   </si>
   <si>
     <t>Honduras</t>
   </si>
   <si>
-    <t>Ministerial</t>
-  </si>
-  <si>
-    <t>SINAGER</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> El Sistema Nacional de Gestión de Riesgos (SINAGER) se
-regulará en un marco institucional, el cual comprenderá a todos los sectores de la sociedad hondureña, tales sectores son el público y el privado. LEY DEL SISTEMA NACIONAL DE GESTIÓN DE RIESGOS (SINAGER)  se definirán, planificarán y ejecutarán todas las acciones relacionadas con la prevención, adaptación al cambio climático y a otro tipo de eventos, manejo financiero del riesgo de desastres, preparación permanente y efectiva, la asistencia de ayuda humanitaria en caso de desastres y emergencia, a la rehabilitación y reconstrucción de las zonas afectadas por desastres.</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=Se-suspenden-labores-en-el-sector-Publico-y-Privado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1)Se suspenden labores en el sector Público y Privado.
-2) Se prohíben eventos de todo tipo y número de personas.
-3) Se cancela toda actividades deportivas, cultural y sociales.
-4) Se prohíbe el funcionamiento del Transporte público.
-5) Se suspenden las celebraciones religiosas presenciales.
-6) Se cierran todos los negocios incluyendo centros comerciales.
-7) Se cierran las fronteras aéreas, terrestres y marítimas en todo el territorio nacional. </t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=Comunicados&amp;page=10</t>
-  </si>
-  <si>
-    <t>Ministerio Público</t>
-  </si>
-  <si>
-    <t>El Ministerio Público (Fiscalía General o Procuraduría) es un organismo Público generalmente estatal, al que se atribuye, dentro de un estado de Derecho democrático la representación de los intereses de la sociedad mediante el ejercicio de las facultades de dirección de la investigación.</t>
-  </si>
-  <si>
-    <t>El Ministerio Público, ante la Alerta Roja para todo el país como medida para evitar el COVID-19 (Coronavirus), INFORMA LO SIGUIENTE:
- Suspender las labores a nivel nacional para todo el personal que labora en las diferentes oficinas desde este lunes 16 de marzo a las 12:00 horas hasta el próximo domingo 22 de marzo a las 23:59:59 horas; Se exceptúa de esa disposición a todo aquel empleado que tengan que desarrollar actividades previas o planificadas con anticipación, tales como: turnos y otras inherentes al normal desempeño de esta Institución.</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=comunicado-del-ministerio-publico</t>
-  </si>
-  <si>
-    <t>16/3/2020</t>
-  </si>
-  <si>
-    <t>La institución que rectora lo concerniente al gobierno del interior de la república, la gobernabilidad, el acceso a la justicia y  la descentralización, contribuyendo a una  cultura democrática, al desarrollo local,  con transparencia y participación ciudadana, para el bienestar social cultural y el honor de la población en general.</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=Comunicados&amp;page=9</t>
-  </si>
-  <si>
-    <t>Ante la emergencia nacional como prevención ante el COVID-19, se realizó la suspensión de labores en dichas Dependencias a partir del lunes dieciséis (16) al viernes veinte (20) de marzo del presente año.
-Los días antes mencionados se declaran INHÁBILES para los efectos, plazos, actuaciones y términos legales que la Ley establece, los cuales quedan suspendidos empezando a correr nuevamente los términos legales a partir del primer día hábil.</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=comunicado-secretaria-de-gobernacion-justicia-y-descentralizacion</t>
-  </si>
-  <si>
-    <t>Agencia Hondureña de Aeronáutica Civil.</t>
-  </si>
-  <si>
-    <t>Agencia encargada de vigilancia y supervisión de las operaciones de aviación civil que se desarrollan en la República de Honduras.</t>
-  </si>
-  <si>
-    <t>En marco de la declaracion de emergencia nacional y las ultimas disposiciones emitidas en el Decreto Ejecutivo PCM -021-2020 en el que se decreta la suspensión  de algunas garantias constitucionales. Se notifica que se dispone el cierre de operaciones de los aeropuertos internacionales.</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=comunicado-aeropuertos-de-honduras</t>
-  </si>
-  <si>
-    <t>17/3/2020</t>
-  </si>
-  <si>
-    <t>Administracion Aduanera de Honduras</t>
-  </si>
-  <si>
-    <t>Institución cuya misión es garantizar la facilitación del comercio, la recaudación y la seguridad mediante un control eficiente, utilizando las mejores prácticas a fin de contribuir al aumento y dinamización de la actividad económica del país.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ante el Decreto Ejecutivo PCM 021-2020 se informa lo siguiente: En aras de facilitar el comercio y el ingreso de suministros, los diferentes puntos aduaneros del país estan operando de manera normal en las actividades de comercio exterior de exportacion e importacion de mercancias. </t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=excepcion-para-puntos-aduaneros</t>
+    <t>Secretaria de Trabajo y Seguridad Social</t>
+  </si>
+  <si>
+    <t>Secretaría de Trabajo y Seguridad Social de Honduras es el encargado de lo concerniente a la formulación, coordinación, ejecución y evaluación de las políticas de empleo, inclusive de los discapacitados, el salario, la formación de mano de obra, el fomento de la educación obrera y de las relaciones obreras patronales, la inmigración laboral selectiva, la coordinación del sistema de Seguridad Social, el reconocimiento y registro de la personalidad jurídica de Sindicatos y demás organizaciones laborales, lo relativo a la higiene y seguridad ocupacional, el manejo de los procedimientos administrativos de solución de los conflictos individuales y colectivos de trabajo.</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=Comunicados&amp;page=6</t>
+  </si>
+  <si>
+    <t>Se autoriza a los empleadores y trabajadores del sector privado para que mediante acuerdo entre las partes convengan que los días feriados señalados en el artículo 339 del Código de Trabajo se consideren como otorgados y gozados por parte de los trabajadores durante el periodo de vigencia del Estado de Emergencia Sanitaria Nacional por la propagación del Covid-19 (Coronavirus).-</t>
+  </si>
+  <si>
+    <t>https://covid19honduras.org/?q=secretaria-de-trabajo</t>
+  </si>
+  <si>
+    <t>26/3/2020</t>
   </si>
   <si>
     <t>Secretaría de Desarrollo Económico</t>
   </si>
   <si>
+    <t>Economía</t>
+  </si>
+  <si>
     <t>Secretaria responsable en fomentar el crecimiento en las inversiones y exportaciones en consonancia con la implementación agresiva de la promoción de la imagen y marca país y, de la competitividad, garantizar el acceso en un 100% a los mercados internacionales y la efectividad del funcionamiento del régimen de comercio exterior, facilitar la gestión empresarial, promover la generación de empleo a través del fomento de la competitividad y productividad de las MIPYMES-SSE y velar por la protección de los consumidores</t>
   </si>
   <si>
-    <t>https://covid19honduras.org/?q=Comunicados&amp;page=8</t>
-  </si>
-  <si>
-    <t>El gobierno de la República, a través de la Secretaria de Desarollo Económico, en el marco de la emergencia nacional sanitaria decretada, informa: Para garantizar que no se comentan abusus contra la población, a nivel nacional se decreta congelamiento de preciosos absoluto de los productos de la canasta básica y productos de higiene personal y de hogar.</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=congelamiento-de-precios-absoluto</t>
-  </si>
-  <si>
-    <t>18/3/2020</t>
-  </si>
-  <si>
-    <t>Instituto Nacional de Migración (INM)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instituto Nacional de Migración tiene como misión fundamental ejercer el control y regulación como máxima autoridad en materia migratoria a nacionales y extranjeros en el marco de la protección de sus derechos y seguridad, en aplicación de la Ley de Migración y Extranjería y la Política Migratoria del Gobierno de la República, mediante una gestión migratoria moderna, dinámica y transparente.
- </t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=Comunicados&amp;page=7</t>
-  </si>
-  <si>
-    <t>Siguiendo las disposiciones emitidas por el gobierno de Honduras el INM informa que los puntos de control migratorio se mantienen operando para: 1) Ingreso al país de hondureños residentes y diplomáticos. 2) Salida del terrotoio nacional a extranjeros. 3) Entrada y salida de transportistas de carga unicamente.</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=flujos-migratorios</t>
-  </si>
-  <si>
-    <t>21/3/2020</t>
-  </si>
-  <si>
-    <t>Comision Nacional de Bancos y Seguro (CNBS)</t>
-  </si>
-  <si>
-    <t>Institución que por mandato constitucional tiene la responsabilidad de velar por la estabilidad y solvencia del sistema financiero y demás supervisados, su regulación, supervisión y control. Asimismo, vigilamos la transparencia y que se respeten los derechos de los usuarios financieros, así como coadyuvamos con el sistema de prevención y detección del lavado activos y financiamiento al terrorismo, y contribuimos a promover la educación e inclusión financiera, a fin de salvaguardar el interés público.</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=cnbs-22-3</t>
-  </si>
-  <si>
-    <t>Las instituciones por la CNBS que realizan operaciones de crédito, podran otorgar periodos de gracia a los deudores que sean afectados por la reduccion de sus flujos de efectivo los cuales se podran otorgar hasta el 30 de junio de 2020.</t>
-  </si>
-  <si>
-    <t>22/3/2020</t>
-  </si>
-  <si>
-    <t>Secretaria de Trabajo y Seguridad Social</t>
-  </si>
-  <si>
-    <t>Secretaría de Trabajo y Seguridad Social de Honduras es el encargado de lo concerniente a la formulación, coordinación, ejecución y evaluación de las políticas de empleo, inclusive de los discapacitados, el salario, la formación de mano de obra, el fomento de la educación obrera y de las relaciones obreras patronales, la inmigración laboral selectiva, la coordinación del sistema de Seguridad Social, el reconocimiento y registro de la personalidad jurídica de Sindicatos y demás organizaciones laborales, lo relativo a la higiene y seguridad ocupacional, el manejo de los procedimientos administrativos de solución de los conflictos individuales y colectivos de trabajo.</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=Comunicados&amp;page=6</t>
-  </si>
-  <si>
-    <t>Se autoriza a los empleadores y trabajadores del sector privado para que mediante acuerdo entre las partes convengan que los días feriados señalados en el artículo 339 del Código de Trabajo se consideren como otorgados y gozados por parte de los trabajadores durante el periodo de vigencia del Estado de Emergencia Sanitaria Nacional por la propagación del Covid-19 (Coronavirus).-</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=secretaria-de-trabajo</t>
-  </si>
-  <si>
-    <t>26/3/2020</t>
-  </si>
-  <si>
-    <t>Economía</t>
-  </si>
-  <si>
     <t>https://covid19honduras.org/?q=Comunicados&amp;page=5</t>
   </si>
   <si>
@@ -292,16 +326,16 @@
   </si>
   <si>
     <t>18/4/2020</t>
-  </si>
-  <si>
-    <t>Secretaría de Gobernación Justicia y Desentralización</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,11 +464,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -457,27 +492,21 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -508,34 +537,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="2" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -581,7 +601,29 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -811,6 +853,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="medium">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color theme="4"/>
         </left>
@@ -832,13 +881,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color theme="4"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -938,8 +980,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K14" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:K14" xr:uid="{EAF3A26F-8D4B-46F0-8F27-A70184B410C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K15" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:K15" xr:uid="{EAF3A26F-8D4B-46F0-8F27-A70184B410C1}"/>
   <tableColumns count="11">
     <tableColumn id="2" xr3:uid="{A60CF310-D129-4744-AE47-EA0A16C6004B}" name="Fuente" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{CC100997-5BD5-48A6-8DA1-3E422557046E}" name="ID_Dato " dataDxfId="9">
@@ -952,15 +994,15 @@
     <tableColumn id="10" xr3:uid="{C428BE36-6D12-4F4C-937B-4D9B2BE733CB}" name="Sitio Web" dataDxfId="4"/>
     <tableColumn id="14" xr3:uid="{8A64974B-7039-4EC2-86FD-F906B25B65C5}" name="Fecha consulta" dataDxfId="3"/>
     <tableColumn id="15" xr3:uid="{76A5A7F7-E8CD-4AD7-BD38-521CEC7FA43D}" name="Fecha publicación" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{C1BACFD5-672A-458F-A24A-AF2164F6B966}" name="País" dataDxfId="0"/>
-    <tableColumn id="17" xr3:uid="{CBA3644C-97A1-4B18-A3FF-89F9754FAC27}" name="División administrativa" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{C1BACFD5-672A-458F-A24A-AF2164F6B966}" name="País" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{CBA3644C-97A1-4B18-A3FF-89F9754FAC27}" name="División administrativa" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1256,27 +1298,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355F3C84-FBC8-4F70-8922-1A1A2826C9C6}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="69.109375" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
-    <col min="6" max="6" width="55.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="69.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="55.28515625" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
-    <col min="11" max="11" width="22.5546875" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="31.9" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1311,8 +1353,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:12" ht="84.75" customHeight="1">
+      <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="6">
@@ -1322,21 +1364,21 @@
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>14</v>
+      <c r="G2" s="24" t="s">
+        <v>16</v>
       </c>
       <c r="H2" s="7"/>
-      <c r="I2" s="4" t="s">
-        <v>16</v>
+      <c r="I2" s="7">
+        <v>44140</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>17</v>
@@ -1346,32 +1388,32 @@
       </c>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:12" ht="85.5" customHeight="1">
+      <c r="A3" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="6">
-        <f t="shared" ref="B3:B7" si="0">+ROW()-1</f>
+        <f t="shared" ref="B3:B8" si="0">+ROW()-1</f>
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="D3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="E3" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="F3" s="10" t="s">
         <v>23</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>24</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>17</v>
@@ -1381,32 +1423,32 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>24</v>
+    <row r="4" spans="1:12" ht="89.25" customHeight="1">
+      <c r="A4" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="B4" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="4" t="s">
+      <c r="D4" s="9" t="s">
         <v>28</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="12"/>
+      <c r="I4" s="7">
+        <v>44079</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>17</v>
@@ -1415,205 +1457,201 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>80</v>
+    <row r="5" spans="1:12" ht="87" customHeight="1">
+      <c r="A5" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="B5" s="6">
-        <f t="shared" si="0"/>
+        <f>+ROW()-1</f>
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="25"/>
+      <c r="I5" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>33</v>
+    <row r="6" spans="1:12" ht="98.25" customHeight="1">
+      <c r="A6" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="B6" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="8"/>
+      <c r="F6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="12"/>
       <c r="I6" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="69" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>38</v>
+    <row r="7" spans="1:12" ht="135">
+      <c r="A7" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="B7" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="4" t="s">
-        <v>37</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="12"/>
+      <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="5"/>
+      <c r="K7" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>42</v>
+    <row r="8" spans="1:12" ht="90">
+      <c r="A8" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="B8" s="6">
-        <f t="shared" ref="B8:B12" si="1">+ROW()-1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="14"/>
+      <c r="D8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="12"/>
       <c r="I8" s="4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>48</v>
+    <row r="9" spans="1:12" ht="120">
+      <c r="A9" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="B9" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B9:B13" si="1">+ROW()-1</f>
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" s="14"/>
+      <c r="D9" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="12"/>
       <c r="I9" s="4" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>54</v>
+    <row r="10" spans="1:12" ht="158.25" customHeight="1">
+      <c r="A10" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="B10" s="6">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>53</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="12"/>
       <c r="I10" s="4" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>59</v>
+    <row r="11" spans="1:12" ht="105">
+      <c r="A11" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="B11" s="6">
         <f t="shared" si="1"/>
@@ -1622,160 +1660,196 @@
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" s="14"/>
+      <c r="D11" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>69</v>
+      </c>
       <c r="I11" s="4" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="16">
+    <row r="12" spans="1:12" ht="150">
+      <c r="A12" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="6">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="C12" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="J12" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" s="21"/>
+      <c r="C12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="12"/>
+      <c r="I12" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:12" ht="120">
+      <c r="A13" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="14">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="18"/>
+      <c r="I13" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="J13" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="6">
-        <f t="shared" ref="B13:B14" si="2">+ROW()-1</f>
+      <c r="K13" s="19"/>
+    </row>
+    <row r="14" spans="1:12" ht="63.75">
+      <c r="A14" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="6">
+        <f t="shared" ref="B14:B15" si="2">+ROW()-1</f>
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" ht="150">
+      <c r="A15" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="6">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" s="5"/>
-    </row>
-    <row r="14" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="6">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G14" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14" s="5"/>
+      <c r="E15" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="H15" s="12"/>
+      <c r="I15" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K15" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada no válida" error="Selecciona una categoría de la lista" promptTitle="Categoria" prompt="Selecciona una categoría de la lista" sqref="C2:C14" xr:uid="{6886B6D6-D01B-4A3E-AC32-C93F79577E67}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada no válida" error="Selecciona una categoría de la lista" promptTitle="Categoria" prompt="Selecciona una categoría de la lista" sqref="C2:C15" xr:uid="{6886B6D6-D01B-4A3E-AC32-C93F79577E67}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{89832B8C-46B1-4E3A-B226-0588FB37741C}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{44E5BE55-9BE8-4C19-8EB2-4729F3ABC777}"/>
-    <hyperlink ref="G3" r:id="rId3" xr:uid="{83338F0A-2385-4D32-BE92-53C6E626689D}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{2AEE38DF-B0A8-494B-AD95-04F5680089A1}"/>
-    <hyperlink ref="G4" r:id="rId5" xr:uid="{CE613E8D-42BF-4A3B-8E64-31449DCA5FFB}"/>
-    <hyperlink ref="E4" r:id="rId6" xr:uid="{90C4CEF0-1AA8-4543-8251-15693CDFF9B6}"/>
-    <hyperlink ref="G5" r:id="rId7" xr:uid="{4E4760D3-6939-4C41-ADE3-E7A46EE0C5BC}"/>
-    <hyperlink ref="E5" r:id="rId8" xr:uid="{76EDB031-9D13-49CF-A7FB-527CC4D7B499}"/>
-    <hyperlink ref="G6" r:id="rId9" xr:uid="{C20EEBB6-370E-4FE3-B260-271A29AF1401}"/>
-    <hyperlink ref="E6" r:id="rId10" xr:uid="{DCBF52A4-8079-4083-8EFA-355A40E5133C}"/>
-    <hyperlink ref="G7" r:id="rId11" xr:uid="{27ED4CFC-A676-49E3-8DBF-B96D8241FED5}"/>
-    <hyperlink ref="E7" r:id="rId12" xr:uid="{D1755C3C-47A5-4BE1-9969-B7EF3A410A83}"/>
-    <hyperlink ref="G8" r:id="rId13" xr:uid="{90448276-2029-41D4-9F26-EDF75765AFE7}"/>
-    <hyperlink ref="E8" r:id="rId14" xr:uid="{61140C4B-261F-49F4-A165-F05ECDA09000}"/>
-    <hyperlink ref="G9" r:id="rId15" xr:uid="{B333F99D-E6A3-441B-91B8-5644745830C4}"/>
-    <hyperlink ref="E9" r:id="rId16" xr:uid="{52316D1F-F875-45D4-BC68-D0EF12900E9A}"/>
-    <hyperlink ref="G10" r:id="rId17" xr:uid="{F2765C1B-000B-42B0-B842-3A1C402875AF}"/>
-    <hyperlink ref="E10" r:id="rId18" xr:uid="{BF4AAFF6-8642-42F4-B4D4-D27AEF285F0C}"/>
-    <hyperlink ref="G11" r:id="rId19" xr:uid="{90EAA1B8-67AE-4786-9AB7-EFFE2A7274E9}"/>
-    <hyperlink ref="E11" r:id="rId20" xr:uid="{16313C5E-575A-4E7B-9020-293E4E52A652}"/>
-    <hyperlink ref="G12" r:id="rId21" xr:uid="{7245FDFD-2CBD-47B4-93DF-91FF93243F7E}"/>
-    <hyperlink ref="E12" r:id="rId22" xr:uid="{D11C0F98-DCAB-4BBA-A8DC-4E2B66805B18}"/>
-    <hyperlink ref="G13" r:id="rId23" xr:uid="{8C650575-6C55-44BD-A0BA-59EFE971353F}"/>
-    <hyperlink ref="E13" r:id="rId24" xr:uid="{B0E6EF00-013B-46E0-A9D8-D76A7488E3F0}"/>
-    <hyperlink ref="G14" r:id="rId25" xr:uid="{D888ED92-439A-42B0-91EF-7BD2E8F09DE8}"/>
-    <hyperlink ref="E14" r:id="rId26" xr:uid="{249E9D6C-C4E9-48FF-89C0-9FE1AC968A21}"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{2AEE38DF-B0A8-494B-AD95-04F5680089A1}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{90C4CEF0-1AA8-4543-8251-15693CDFF9B6}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{DCBF52A4-8079-4083-8EFA-355A40E5133C}"/>
+    <hyperlink ref="E8" r:id="rId4" xr:uid="{D1755C3C-47A5-4BE1-9969-B7EF3A410A83}"/>
+    <hyperlink ref="G9" r:id="rId5" xr:uid="{90448276-2029-41D4-9F26-EDF75765AFE7}"/>
+    <hyperlink ref="E9" r:id="rId6" xr:uid="{61140C4B-261F-49F4-A165-F05ECDA09000}"/>
+    <hyperlink ref="G10" r:id="rId7" xr:uid="{B333F99D-E6A3-441B-91B8-5644745830C4}"/>
+    <hyperlink ref="G11" r:id="rId8" xr:uid="{F2765C1B-000B-42B0-B842-3A1C402875AF}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{BF4AAFF6-8642-42F4-B4D4-D27AEF285F0C}"/>
+    <hyperlink ref="G12" r:id="rId10" xr:uid="{90EAA1B8-67AE-4786-9AB7-EFFE2A7274E9}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{16313C5E-575A-4E7B-9020-293E4E52A652}"/>
+    <hyperlink ref="G13" r:id="rId12" xr:uid="{7245FDFD-2CBD-47B4-93DF-91FF93243F7E}"/>
+    <hyperlink ref="E13" r:id="rId13" xr:uid="{D11C0F98-DCAB-4BBA-A8DC-4E2B66805B18}"/>
+    <hyperlink ref="G14" r:id="rId14" xr:uid="{8C650575-6C55-44BD-A0BA-59EFE971353F}"/>
+    <hyperlink ref="E14" r:id="rId15" xr:uid="{B0E6EF00-013B-46E0-A9D8-D76A7488E3F0}"/>
+    <hyperlink ref="G15" r:id="rId16" xr:uid="{D888ED92-439A-42B0-91EF-7BD2E8F09DE8}"/>
+    <hyperlink ref="E15" r:id="rId17" xr:uid="{249E9D6C-C4E9-48FF-89C0-9FE1AC968A21}"/>
+    <hyperlink ref="G2" r:id="rId18" xr:uid="{967C671C-6223-4E72-95EB-848FCA4ED0AA}"/>
+    <hyperlink ref="G3" r:id="rId19" xr:uid="{A95EBDBE-7BE2-4CD1-9893-147DD330BDEC}"/>
+    <hyperlink ref="G4" r:id="rId20" xr:uid="{12882DD5-C454-4AF2-B5EC-A9B985CD566B}"/>
+    <hyperlink ref="E6" r:id="rId21" xr:uid="{D9D9F19F-7736-4860-BAF8-DA16E8624C87}"/>
+    <hyperlink ref="E2" r:id="rId22" xr:uid="{86D8BCBE-AE34-4369-AC21-ABBEED56327A}"/>
+    <hyperlink ref="G6" r:id="rId23" xr:uid="{AC0E852D-23E0-41D9-B0F1-DDA2F1296DC6}"/>
+    <hyperlink ref="G7" r:id="rId24" xr:uid="{28A1FB3E-AFD1-443D-AC97-010941BE206C}"/>
+    <hyperlink ref="G8" r:id="rId25" xr:uid="{920C3700-75B1-488F-8021-EA494D4E2884}"/>
+    <hyperlink ref="G5" r:id="rId26" xr:uid="{95A6F2F1-4E35-44D8-8C0C-BF6C8CD37D74}"/>
+    <hyperlink ref="E5" r:id="rId27" xr:uid="{A863AB1D-5AF0-49BC-B740-B618B0C20E37}"/>
+    <hyperlink ref="E10" r:id="rId28" xr:uid="{975ACC32-AA5A-4C4F-A55A-F7672D47DA59}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId27"/>
+    <tablePart r:id="rId29"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 05-14-2020 19-03-54
</commit_message>
<xml_diff>
--- a/datacovidgt/00 DATACOVID Trabajo_GT.xlsx
+++ b/datacovidgt/00 DATACOVID Trabajo_GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="338" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2779D902-425F-48FD-9820-9BD06B169BEE}"/>
+  <xr:revisionPtr revIDLastSave="359" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ED3C2E99-13F4-420A-A093-7B9E59235B97}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56D738C3-148A-420A-8894-4D7B344C02BA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72">
   <si>
     <t>Fuente</t>
   </si>
@@ -74,28 +74,28 @@
     <t>División administrativa</t>
   </si>
   <si>
-    <t>Organismo Judicial</t>
+    <t>Ministerio de Trabajo y Previsión Social</t>
   </si>
   <si>
     <t>Trabajo</t>
   </si>
   <si>
-    <t>Conforme lo establece la Constitución Política de la República de Guatemala, el Organismo Judicial es el encargado de impartir justicia, con independencia y potestad de juzgar. La Ley del Organismo Judicial cita que en ejercicio de la soberanía delegada por el pueblo, imparte justicia en concordancia con el texto constitucional.</t>
-  </si>
-  <si>
-    <t>https://legal.dca.gob.gt/GestionDocumento/VisualizarDocumento?verDocumentoPrevia=True&amp;versionImpresa=False&amp;doc=59663</t>
-  </si>
-  <si>
-    <t>Se amplia suspensión de las labores de los organismos juridisccionales y administrativas del 12 al 18 de mayo de 2020, inclusive, extendiendose ésta como licencia con goce de salario para todo el personal administratvio y judicial</t>
-  </si>
-  <si>
-    <t>http://www.oj.gob.gt/</t>
+    <t>El Ministerio de Trabajo y Previsión Social de la República de Guatemala (MINTRAB), es la institución estatal encargada de velar y promover el cumplimiento eficiente y eficaz de la legislación, políticas y programas relativos al trabajo y la previsión social, en beneficio de la sociedad y busca ser un Ministerio que promueva la cultura de respeto a la legislación laboral y el bienestar de la sociedad.</t>
+  </si>
+  <si>
+    <t>https://www.mintrabajo.gob.gt/images/Publicaciones/Coronavirus/Acuerdo_Ministerial_140-2020.pdf</t>
+  </si>
+  <si>
+    <t>Normativa para suspensión de contrados de trabajo por mergencia del COVID-19</t>
+  </si>
+  <si>
+    <t>https://www.mintrabajo.gob.gt/</t>
+  </si>
+  <si>
+    <t>23/3/2020</t>
   </si>
   <si>
     <t>Guatemala</t>
-  </si>
-  <si>
-    <t>Ministerial</t>
   </si>
   <si>
     <t>Universidad de San Carlos de Guatemala</t>
@@ -122,12 +122,115 @@
     <t>22/3/2020</t>
   </si>
   <si>
+    <t>Ministerial</t>
+  </si>
+  <si>
+    <t>Secretaría General de la Presidencia de la República de Guatemala</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>La Secretaría General de la Presidencia de la República (SGP) es el órgano responsable del apoyo jurídico y administrativo con carácter inmediato y constante del Presidente de la República. Su función es tramitar los asuntos de Gobierno del Despacho del Presidente.</t>
+  </si>
+  <si>
+    <t>https://legal.dca.gob.gt/GestionDocumento/VisualizarDocumento?verDocumentoPrevia=True&amp;versionImpresa=False&amp;doc=59265</t>
+  </si>
+  <si>
+    <t>Prórroga del Estado de Calamidad Pública y órdenes para el estricto cumplimiento</t>
+  </si>
+  <si>
+    <t>https://sgp.gob.gt/</t>
+  </si>
+  <si>
+    <t>20/04/2020</t>
+  </si>
+  <si>
+    <t>Superintendencia de Bancos</t>
+  </si>
+  <si>
+    <t>Financiero</t>
+  </si>
+  <si>
+    <t>La Superintendencia de Bancos de Guatemala, (SIB), organizada conforme a la ley, es el órgano que ejercerá la vigilancia e inspección de bancos, instituciones de crédito, empresas financieras, entidades afianzadoras, de seguros y las demás que la ley disponga.</t>
+  </si>
+  <si>
+    <t>https://www.sib.gob.gt/web/sib/inicio</t>
+  </si>
+  <si>
+    <t>Medidas temporales especiales para atender la coyuntura
+derivada de la pandemia denominada COVID-19, que pueden ser observadas por las instituciones supervisadas por la Superintendencia de Bancos que otorgan financiamiento</t>
+  </si>
+  <si>
+    <t>file:///C:/Users/MARN%201/Downloads/JM-32-2020%20Para%20atender%20la%20coyuntura%20derivada%20de%20la%20pandemia%20denominada%20COVID-19.pdf</t>
+  </si>
+  <si>
+    <t>19/3/2020</t>
+  </si>
+  <si>
+    <t>Disposiciones Presidenciales en caso de calamidad pública</t>
+  </si>
+  <si>
+    <t>https://www.mintrabajo.gob.gt/images/Publicaciones/Coronavirus/Decreto_Gubernativo_No._5-2020.pdf</t>
+  </si>
+  <si>
+    <t>16/3/2020</t>
+  </si>
+  <si>
+    <t>Ministerio de Economica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Ministerio de Economía (MINECO) es el ministerio del Gobierno de Guatemala encargado de hacer cumplir el régimen jurídico relativo al desarrollo de las actividades productivas no agropecuarias, del comercio interno y externo, de la protección al consumidor, del fomento a la competencia, de la represión legal de la competencia desleal, de la limitación al funcionamiento de empresas monopólicas; de inversión nacional y extranjera, de promoción a la competitividad, del desarrollo industrial y comercial. </t>
+  </si>
+  <si>
+    <t>https://www.mineco.gob.gt/</t>
+  </si>
+  <si>
+    <t>Reglamento para el Otorgamiento del Beneficio del Fondo para la Protección del Empleo</t>
+  </si>
+  <si>
+    <t>https://www.mintrabajo.gob.gt/images/Publicaciones/Coronavirus/Reglamento_Fondo_Protec_Empleo_-_Acdo_Gub_58-2020.pdf</t>
+  </si>
+  <si>
+    <t>Ministerio de Salud Pública</t>
+  </si>
+  <si>
+    <t>Salud</t>
+  </si>
+  <si>
+    <t>El Ministerio de Salud Pública y Asistencia Social de la República de Guatemala (MSPAS) le corresponde formular las políticas y hacer cumplir el régimen jurídico relativo a la salud preventiva y curativa y a las acciones de protección, promoción, recuperación y rehabilitación de la salud física y mental de los habitantes del país y a la preservación higiénica de medio ambiente; a la orientación y coordinación de la cooperación técnica y financiera en salud y a velar por el cumplimiento de los tratados y convenios internacionales relacionados con la salud en casos de emergencias por epidemias y desastres naturales; y, a regir en forma descentralizada el sistema de capacitación y formulación de los recursos humanos del sector salud.</t>
+  </si>
+  <si>
+    <t>https://www.mspas.gob.gt/</t>
+  </si>
+  <si>
+    <t>Reorganización de personal. Para dar cumplimiento a las disposiciones emanadas en el Decreto Gubernativo Número 5-2020 .Estado de Calamidad Publica</t>
+  </si>
+  <si>
+    <t>https://www.mspas.gob.gt/index.php/component/jdownloads/send/420-2020/3404-acuerdo-ministerial-no-55-2020</t>
+  </si>
+  <si>
+    <t>16/03/2020</t>
+  </si>
+  <si>
+    <t>Organismo Judicial</t>
+  </si>
+  <si>
+    <t>Conforme lo establece la Constitución Política de la República de Guatemala, el Organismo Judicial es el encargado de impartir justicia, con independencia y potestad de juzgar. La Ley del Organismo Judicial cita que en ejercicio de la soberanía delegada por el pueblo, imparte justicia en concordancia con el texto constitucional.</t>
+  </si>
+  <si>
+    <t>https://legal.dca.gob.gt/GestionDocumento/VisualizarDocumento?verDocumentoPrevia=True&amp;versionImpresa=False&amp;doc=59663</t>
+  </si>
+  <si>
+    <t>Se amplia suspensión de las labores de los organismos juridisccionales y administrativas del 12 al 18 de mayo de 2020, inclusive, extendiendose ésta como licencia con goce de salario para todo el personal administratvio y judicial</t>
+  </si>
+  <si>
+    <t>http://www.oj.gob.gt/</t>
+  </si>
+  <si>
     <t>Congreso Nacional de la República de Guatemala</t>
   </si>
   <si>
-    <t>General</t>
-  </si>
-  <si>
     <t>El Organismo Legislativo de la República de Guatemala (OL) es uno de los organismos del Estado, que ejerce el poder legislativo. Es decir, que tiene la potestad legislativa para hacer las leyes que favorezcan al desarrollo integral del país, así como, procurar el bienestar común entre los habitantes. Está compuesto por los diputados del Congreso de la República y por el personal técnico y administrativo.</t>
   </si>
   <si>
@@ -138,33 +241,6 @@
   </si>
   <si>
     <t>https://www.congreso.gob.gt/</t>
-  </si>
-  <si>
-    <t>Secretaría General de la Presidencia de la República de Guatemala</t>
-  </si>
-  <si>
-    <t>La Secretaría General de la Presidencia de la República (SGP) es el órgano responsable del apoyo jurídico y administrativo con carácter inmediato y constante del Presidente de la República. Su función es tramitar los asuntos de Gobierno del Despacho del Presidente.</t>
-  </si>
-  <si>
-    <t>https://legal.dca.gob.gt/GestionDocumento/VisualizarDocumento?verDocumentoPrevia=True&amp;versionImpresa=False&amp;doc=59265</t>
-  </si>
-  <si>
-    <t>Disposiciones Presidenciales en caso de calamidad pública</t>
-  </si>
-  <si>
-    <t>https://www.mintrabajo.gob.gt/images/Publicaciones/Coronavirus/Decreto_Gubernativo_No._5-2020.pdf</t>
-  </si>
-  <si>
-    <t>16/3/2020</t>
-  </si>
-  <si>
-    <t>Prórroga del Estado de Calamidad Pública y órdenes para el estricto cumplimiento</t>
-  </si>
-  <si>
-    <t>https://sgp.gob.gt/</t>
-  </si>
-  <si>
-    <t>20/04/2020</t>
   </si>
   <si>
     <t>Superintendencia de Administracion Tributaria</t>
@@ -184,148 +260,6 @@
   </si>
   <si>
     <t>https://portal.sat.gob.gt/portal/</t>
-  </si>
-  <si>
-    <t>Ministerio de Trabajo y Previsión Social</t>
-  </si>
-  <si>
-    <t>El Ministerio de Trabajo y Previsión Social de la República de Guatemala (MINTRAB), es la institución estatal encargada de velar y promover el cumplimiento eficiente y eficaz de la legislación, políticas y programas relativos al trabajo y la previsión social, en beneficio de la sociedad y busca ser un Ministerio que promueva la cultura de respeto a la legislación laboral y el bienestar de la sociedad.</t>
-  </si>
-  <si>
-    <t>https://www.mintrabajo.gob.gt/images/Publicaciones/Coronavirus/Acuerdo_Ministerial_140-2020.pdf</t>
-  </si>
-  <si>
-    <t>Normativa para suspensión de contrados de trabajo por mergencia del COVID-19</t>
-  </si>
-  <si>
-    <t>https://www.mintrabajo.gob.gt/</t>
-  </si>
-  <si>
-    <t>23/3/2020</t>
-  </si>
-  <si>
-    <t>Ministerio de Economica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El Ministerio de Economía (MINECO) es el ministerio del Gobierno de Guatemala encargado de hacer cumplir el régimen jurídico relativo al desarrollo de las actividades productivas no agropecuarias, del comercio interno y externo, de la protección al consumidor, del fomento a la competencia, de la represión legal de la competencia desleal, de la limitación al funcionamiento de empresas monopólicas; de inversión nacional y extranjera, de promoción a la competitividad, del desarrollo industrial y comercial. </t>
-  </si>
-  <si>
-    <t>https://www.mineco.gob.gt/</t>
-  </si>
-  <si>
-    <t>Reglamento para el Otorgamiento del Beneficio del Fondo para la Protección del Empleo</t>
-  </si>
-  <si>
-    <t>https://www.mintrabajo.gob.gt/images/Publicaciones/Coronavirus/Reglamento_Fondo_Protec_Empleo_-_Acdo_Gub_58-2020.pdf</t>
-  </si>
-  <si>
-    <t>Superintendencia de Bancos</t>
-  </si>
-  <si>
-    <t>Financiero</t>
-  </si>
-  <si>
-    <t>La Superintendencia de Bancos de Guatemala, (SIB), organizada conforme a la ley, es el órgano que ejercerá la vigilancia e inspección de bancos, instituciones de crédito, empresas financieras, entidades afianzadoras, de seguros y las demás que la ley disponga.</t>
-  </si>
-  <si>
-    <t>https://www.sib.gob.gt/</t>
-  </si>
-  <si>
-    <t>Medidas temporales especiales para atender la coyuntura
-derivada de la pandemia denominada COVID-19, que pueden ser observadas por las instituciones supervisadas por la Superintendencia de Bancos que otorgan financiamiento</t>
-  </si>
-  <si>
-    <t>file:///C:/Users/MARN%201/Downloads/JM-32-2020%20Para%20atender%20la%20coyuntura%20derivada%20de%20la%20pandemia%20denominada%20COVID-19.pdf</t>
-  </si>
-  <si>
-    <t>19/3/2020</t>
-  </si>
-  <si>
-    <t>Comision Nacional de Bancos y Seguro (CNBS)</t>
-  </si>
-  <si>
-    <t>Institución que por mandato constitucional tiene la responsabilidad de velar por la estabilidad y solvencia del sistema financiero y demás supervisados, su regulación, supervisión y control. Asimismo, vigilamos la transparencia y que se respeten los derechos de los usuarios financieros, así como coadyuvamos con el sistema de prevención y detección del lavado activos y financiamiento al terrorismo, y contribuimos a promover la educación e inclusión financiera, a fin de salvaguardar el interés público.</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=cnbs-22-3</t>
-  </si>
-  <si>
-    <t>Las instituciones por la CNBS que realizan operaciones de crédito, podran otorgar periodos de gracia a los deudores que sean afectados por la reduccion de sus flujos de efectivo los cuales se podran otorgar hasta el 30 de junio de 2020.</t>
-  </si>
-  <si>
-    <t>21/3/2020</t>
-  </si>
-  <si>
-    <t>Honduras</t>
-  </si>
-  <si>
-    <t>Secretaria de Trabajo y Seguridad Social</t>
-  </si>
-  <si>
-    <t>Secretaría de Trabajo y Seguridad Social de Honduras es el encargado de lo concerniente a la formulación, coordinación, ejecución y evaluación de las políticas de empleo, inclusive de los discapacitados, el salario, la formación de mano de obra, el fomento de la educación obrera y de las relaciones obreras patronales, la inmigración laboral selectiva, la coordinación del sistema de Seguridad Social, el reconocimiento y registro de la personalidad jurídica de Sindicatos y demás organizaciones laborales, lo relativo a la higiene y seguridad ocupacional, el manejo de los procedimientos administrativos de solución de los conflictos individuales y colectivos de trabajo.</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=Comunicados&amp;page=6</t>
-  </si>
-  <si>
-    <t>Se autoriza a los empleadores y trabajadores del sector privado para que mediante acuerdo entre las partes convengan que los días feriados señalados en el artículo 339 del Código de Trabajo se consideren como otorgados y gozados por parte de los trabajadores durante el periodo de vigencia del Estado de Emergencia Sanitaria Nacional por la propagación del Covid-19 (Coronavirus).-</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=secretaria-de-trabajo</t>
-  </si>
-  <si>
-    <t>26/3/2020</t>
-  </si>
-  <si>
-    <t>Secretaría de Desarrollo Económico</t>
-  </si>
-  <si>
-    <t>Economía</t>
-  </si>
-  <si>
-    <t>Secretaria responsable en fomentar el crecimiento en las inversiones y exportaciones en consonancia con la implementación agresiva de la promoción de la imagen y marca país y, de la competitividad, garantizar el acceso en un 100% a los mercados internacionales y la efectividad del funcionamiento del régimen de comercio exterior, facilitar la gestión empresarial, promover la generación de empleo a través del fomento de la competitividad y productividad de las MIPYMES-SSE y velar por la protección de los consumidores</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=Comunicados&amp;page=5</t>
-  </si>
-  <si>
-    <t>Establecer el precio máximo en todo el territorio nacional de los productos al consumidor final.</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=precios-maximos-canasta-basica</t>
-  </si>
-  <si>
-    <t>27/3/2020</t>
-  </si>
-  <si>
-    <t>BANHPROVI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Economía </t>
-  </si>
-  <si>
-    <t>Institución financiera que contribuye al desarrollo socioeconómico del país y al mejoramiento de la calidad de vida de los hondureños, fomentando y fortaleciendo la inclusión financiera de los beneficiarios.</t>
-  </si>
-  <si>
-    <t>Se realizará la readecuación de todos los préstamos redescontados a las instituciones financieras, mediante el traslado de las cuotas de los meses de marzo, abril y mayo de 2020 creando una ampliación de la fecha de vencimiento del crédito.</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=banhprovi</t>
-  </si>
-  <si>
-    <t>24/3/2020</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=Comunicados&amp;page=1</t>
-  </si>
-  <si>
-    <t>Las Empresas que decidan acogerse a las disposiciones de la sección séptima del Decreto Legislativo No. 33-2020, deberán enviar una nota al correo electrónico.</t>
-  </si>
-  <si>
-    <t>https://covid19honduras.org/?q=ley-de-auxilio</t>
-  </si>
-  <si>
-    <t>18/4/2020</t>
   </si>
 </sst>
 </file>
@@ -403,7 +337,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -450,26 +384,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="4"/>
-      </left>
-      <right style="thin">
-        <color theme="4"/>
-      </right>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -501,58 +421,24 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink" xfId="2" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
@@ -980,8 +866,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K15" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:K15" xr:uid="{EAF3A26F-8D4B-46F0-8F27-A70184B410C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K11" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:K11" xr:uid="{EAF3A26F-8D4B-46F0-8F27-A70184B410C1}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K11">
+    <sortCondition descending="1" ref="I1:I11"/>
+  </sortState>
   <tableColumns count="11">
     <tableColumn id="2" xr3:uid="{A60CF310-D129-4744-AE47-EA0A16C6004B}" name="Fuente" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{CC100997-5BD5-48A6-8DA1-3E422557046E}" name="ID_Dato " dataDxfId="9">
@@ -1300,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355F3C84-FBC8-4F70-8922-1A1A2826C9C6}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -1367,25 +1256,23 @@
       <c r="D2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="12" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7">
-        <v>44140</v>
+      <c r="H2" s="11"/>
+      <c r="I2" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="K2" s="5"/>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="85.5" customHeight="1">
@@ -1393,7 +1280,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="6">
-        <f t="shared" ref="B3:B8" si="0">+ROW()-1</f>
+        <f>+ROW()-1</f>
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1402,13 +1289,13 @@
       <c r="D3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="12" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="7"/>
@@ -1416,440 +1303,306 @@
         <v>25</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="89.25" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" s="6">
-        <f t="shared" si="0"/>
+        <f>+ROW()-1</f>
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="23" t="s">
         <v>29</v>
       </c>
+      <c r="E4" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="F4" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="7">
-        <v>44079</v>
+      <c r="G4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:12" ht="87" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B5" s="6">
         <f>+ROW()-1</f>
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:12" ht="98.25" customHeight="1">
       <c r="A6" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B6" s="6">
-        <f t="shared" si="0"/>
+        <f>+ROW()-1</f>
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>34</v>
+        <v>29</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="14"/>
+      <c r="I6" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="135">
+    <row r="7" spans="1:12" ht="120">
       <c r="A7" s="8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B7" s="6">
-        <f t="shared" si="0"/>
+        <f>+ROW()-1</f>
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:12" ht="90">
+    <row r="8" spans="1:12" ht="165">
       <c r="A8" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B8" s="6">
-        <f t="shared" si="0"/>
+        <f>+ROW()-1</f>
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="12"/>
+        <v>53</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="11"/>
       <c r="I8" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="120">
+    <row r="9" spans="1:12" ht="75">
       <c r="A9" s="8" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B9" s="6">
-        <f t="shared" ref="B9:B13" si="1">+ROW()-1</f>
+        <f>+ROW()-1</f>
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="4" t="s">
-        <v>37</v>
+        <v>59</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7">
+        <v>44140</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="158.25" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B10" s="6">
-        <f t="shared" si="1"/>
+        <f>+ROW()-1</f>
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="G10" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="11"/>
+      <c r="I10" s="7">
+        <v>44079</v>
+      </c>
       <c r="J10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" ht="105">
+    <row r="11" spans="1:12" ht="135">
       <c r="A11" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B11" s="6">
-        <f t="shared" si="1"/>
+        <f>+ROW()-1</f>
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>69</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>25</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="K11" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="12" spans="1:12" ht="150">
-      <c r="A12" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="6">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="K12" s="5"/>
-    </row>
-    <row r="13" spans="1:12" ht="120">
-      <c r="A13" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B13" s="14">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="J13" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="K13" s="19"/>
-    </row>
-    <row r="14" spans="1:12" ht="63.75">
-      <c r="A14" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="6">
-        <f t="shared" ref="B14:B15" si="2">+ROW()-1</f>
-        <v>13</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:12" ht="150">
-      <c r="A15" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="6">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="H15" s="12"/>
-      <c r="I15" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="K15" s="5"/>
-    </row>
+    <row r="12" spans="1:12" ht="15"/>
+    <row r="13" spans="1:12" ht="15"/>
+    <row r="14" spans="1:12" ht="15"/>
+    <row r="15" spans="1:12" ht="15"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada no válida" error="Selecciona una categoría de la lista" promptTitle="Categoria" prompt="Selecciona una categoría de la lista" sqref="C2:C15" xr:uid="{6886B6D6-D01B-4A3E-AC32-C93F79577E67}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada no válida" error="Selecciona una categoría de la lista" promptTitle="Categoria" prompt="Selecciona una categoría de la lista" sqref="C2:C11" xr:uid="{6886B6D6-D01B-4A3E-AC32-C93F79577E67}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{2AEE38DF-B0A8-494B-AD95-04F5680089A1}"/>
-    <hyperlink ref="E4" r:id="rId2" xr:uid="{90C4CEF0-1AA8-4543-8251-15693CDFF9B6}"/>
-    <hyperlink ref="E7" r:id="rId3" xr:uid="{DCBF52A4-8079-4083-8EFA-355A40E5133C}"/>
-    <hyperlink ref="E8" r:id="rId4" xr:uid="{D1755C3C-47A5-4BE1-9969-B7EF3A410A83}"/>
-    <hyperlink ref="G9" r:id="rId5" xr:uid="{90448276-2029-41D4-9F26-EDF75765AFE7}"/>
-    <hyperlink ref="E9" r:id="rId6" xr:uid="{61140C4B-261F-49F4-A165-F05ECDA09000}"/>
-    <hyperlink ref="G10" r:id="rId7" xr:uid="{B333F99D-E6A3-441B-91B8-5644745830C4}"/>
-    <hyperlink ref="G11" r:id="rId8" xr:uid="{F2765C1B-000B-42B0-B842-3A1C402875AF}"/>
-    <hyperlink ref="E11" r:id="rId9" xr:uid="{BF4AAFF6-8642-42F4-B4D4-D27AEF285F0C}"/>
-    <hyperlink ref="G12" r:id="rId10" xr:uid="{90EAA1B8-67AE-4786-9AB7-EFFE2A7274E9}"/>
-    <hyperlink ref="E12" r:id="rId11" xr:uid="{16313C5E-575A-4E7B-9020-293E4E52A652}"/>
-    <hyperlink ref="G13" r:id="rId12" xr:uid="{7245FDFD-2CBD-47B4-93DF-91FF93243F7E}"/>
-    <hyperlink ref="E13" r:id="rId13" xr:uid="{D11C0F98-DCAB-4BBA-A8DC-4E2B66805B18}"/>
-    <hyperlink ref="G14" r:id="rId14" xr:uid="{8C650575-6C55-44BD-A0BA-59EFE971353F}"/>
-    <hyperlink ref="E14" r:id="rId15" xr:uid="{B0E6EF00-013B-46E0-A9D8-D76A7488E3F0}"/>
-    <hyperlink ref="G15" r:id="rId16" xr:uid="{D888ED92-439A-42B0-91EF-7BD2E8F09DE8}"/>
-    <hyperlink ref="E15" r:id="rId17" xr:uid="{249E9D6C-C4E9-48FF-89C0-9FE1AC968A21}"/>
-    <hyperlink ref="G2" r:id="rId18" xr:uid="{967C671C-6223-4E72-95EB-848FCA4ED0AA}"/>
-    <hyperlink ref="G3" r:id="rId19" xr:uid="{A95EBDBE-7BE2-4CD1-9893-147DD330BDEC}"/>
-    <hyperlink ref="G4" r:id="rId20" xr:uid="{12882DD5-C454-4AF2-B5EC-A9B985CD566B}"/>
-    <hyperlink ref="E6" r:id="rId21" xr:uid="{D9D9F19F-7736-4860-BAF8-DA16E8624C87}"/>
-    <hyperlink ref="E2" r:id="rId22" xr:uid="{86D8BCBE-AE34-4369-AC21-ABBEED56327A}"/>
-    <hyperlink ref="G6" r:id="rId23" xr:uid="{AC0E852D-23E0-41D9-B0F1-DDA2F1296DC6}"/>
-    <hyperlink ref="G7" r:id="rId24" xr:uid="{28A1FB3E-AFD1-443D-AC97-010941BE206C}"/>
-    <hyperlink ref="G8" r:id="rId25" xr:uid="{920C3700-75B1-488F-8021-EA494D4E2884}"/>
-    <hyperlink ref="G5" r:id="rId26" xr:uid="{95A6F2F1-4E35-44D8-8C0C-BF6C8CD37D74}"/>
-    <hyperlink ref="E5" r:id="rId27" xr:uid="{A863AB1D-5AF0-49BC-B740-B618B0C20E37}"/>
-    <hyperlink ref="E10" r:id="rId28" xr:uid="{975ACC32-AA5A-4C4F-A55A-F7672D47DA59}"/>
+    <hyperlink ref="E10" r:id="rId2" xr:uid="{90C4CEF0-1AA8-4543-8251-15693CDFF9B6}"/>
+    <hyperlink ref="E11" r:id="rId3" xr:uid="{DCBF52A4-8079-4083-8EFA-355A40E5133C}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{D1755C3C-47A5-4BE1-9969-B7EF3A410A83}"/>
+    <hyperlink ref="G7" r:id="rId5" xr:uid="{90448276-2029-41D4-9F26-EDF75765AFE7}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{61140C4B-261F-49F4-A165-F05ECDA09000}"/>
+    <hyperlink ref="G5" r:id="rId7" xr:uid="{B333F99D-E6A3-441B-91B8-5644745830C4}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{967C671C-6223-4E72-95EB-848FCA4ED0AA}"/>
+    <hyperlink ref="G3" r:id="rId9" xr:uid="{A95EBDBE-7BE2-4CD1-9893-147DD330BDEC}"/>
+    <hyperlink ref="G10" r:id="rId10" xr:uid="{12882DD5-C454-4AF2-B5EC-A9B985CD566B}"/>
+    <hyperlink ref="E4" r:id="rId11" xr:uid="{D9D9F19F-7736-4860-BAF8-DA16E8624C87}"/>
+    <hyperlink ref="E9" r:id="rId12" xr:uid="{86D8BCBE-AE34-4369-AC21-ABBEED56327A}"/>
+    <hyperlink ref="G4" r:id="rId13" xr:uid="{AC0E852D-23E0-41D9-B0F1-DDA2F1296DC6}"/>
+    <hyperlink ref="G11" r:id="rId14" xr:uid="{28A1FB3E-AFD1-443D-AC97-010941BE206C}"/>
+    <hyperlink ref="G2" r:id="rId15" xr:uid="{920C3700-75B1-488F-8021-EA494D4E2884}"/>
+    <hyperlink ref="G6" r:id="rId16" xr:uid="{95A6F2F1-4E35-44D8-8C0C-BF6C8CD37D74}"/>
+    <hyperlink ref="E6" r:id="rId17" xr:uid="{A863AB1D-5AF0-49BC-B740-B618B0C20E37}"/>
+    <hyperlink ref="E5" r:id="rId18" xr:uid="{975ACC32-AA5A-4C4F-A55A-F7672D47DA59}"/>
+    <hyperlink ref="G8" r:id="rId19" xr:uid="{AF0C6EBD-F612-45E6-9A1F-40A0797CBAF5}"/>
+    <hyperlink ref="E8" r:id="rId20" xr:uid="{0DDB8F11-8156-4600-BB4A-B8C956376579}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId29"/>
+    <tablePart r:id="rId21"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 05-15-2020 19-07-09
</commit_message>
<xml_diff>
--- a/datacovidgt/00 DATACOVID Trabajo_GT.xlsx
+++ b/datacovidgt/00 DATACOVID Trabajo_GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="359" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ED3C2E99-13F4-420A-A093-7B9E59235B97}"/>
+  <xr:revisionPtr revIDLastSave="368" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{57375707-198B-4DB7-83B4-3B190B94BBCC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56D738C3-148A-420A-8894-4D7B344C02BA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="75">
   <si>
     <t>Fuente</t>
   </si>
@@ -260,6 +260,17 @@
   </si>
   <si>
     <t>https://portal.sat.gob.gt/portal/</t>
+  </si>
+  <si>
+    <t>https://legal.dca.gob.gt/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nuevas Disposiciones presidenciales en caso de calamidad pública 
+y órdenes para el estricto cumplimiento
+</t>
+  </si>
+  <si>
+    <t>15/5/2020</t>
   </si>
 </sst>
 </file>
@@ -337,7 +348,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -384,12 +395,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -435,6 +459,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -866,8 +911,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K11" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:K11" xr:uid="{EAF3A26F-8D4B-46F0-8F27-A70184B410C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K12" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:K12" xr:uid="{EAF3A26F-8D4B-46F0-8F27-A70184B410C1}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K11">
     <sortCondition descending="1" ref="I1:I11"/>
   </sortState>
@@ -1189,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355F3C84-FBC8-4F70-8922-1A1A2826C9C6}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -1570,13 +1615,44 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15"/>
+    <row r="12" spans="1:12" ht="60">
+      <c r="A12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="16">
+        <f>+ROW()-1</f>
+        <v>11</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="19"/>
+      <c r="I12" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="21"/>
+    </row>
     <row r="13" spans="1:12" ht="15"/>
     <row r="14" spans="1:12" ht="15"/>
     <row r="15" spans="1:12" ht="15"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada no válida" error="Selecciona una categoría de la lista" promptTitle="Categoria" prompt="Selecciona una categoría de la lista" sqref="C2:C11" xr:uid="{6886B6D6-D01B-4A3E-AC32-C93F79577E67}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada no válida" error="Selecciona una categoría de la lista" promptTitle="Categoria" prompt="Selecciona una categoría de la lista" sqref="C2:C12" xr:uid="{6886B6D6-D01B-4A3E-AC32-C93F79577E67}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{2AEE38DF-B0A8-494B-AD95-04F5680089A1}"/>
@@ -1599,10 +1675,12 @@
     <hyperlink ref="E5" r:id="rId18" xr:uid="{975ACC32-AA5A-4C4F-A55A-F7672D47DA59}"/>
     <hyperlink ref="G8" r:id="rId19" xr:uid="{AF0C6EBD-F612-45E6-9A1F-40A0797CBAF5}"/>
     <hyperlink ref="E8" r:id="rId20" xr:uid="{0DDB8F11-8156-4600-BB4A-B8C956376579}"/>
+    <hyperlink ref="E12" r:id="rId21" xr:uid="{9DCE4B16-82CC-4B45-B72F-C93FE98BEAFB}"/>
+    <hyperlink ref="G12" r:id="rId22" xr:uid="{344E4542-DCF8-411A-926F-C6E068111423}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId21"/>
+    <tablePart r:id="rId23"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 05-25-2020 16-36-16
</commit_message>
<xml_diff>
--- a/datacovidgt/00 DATACOVID Trabajo_GT.xlsx
+++ b/datacovidgt/00 DATACOVID Trabajo_GT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22920"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="368" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{57375707-198B-4DB7-83B4-3B190B94BBCC}"/>
+  <xr:revisionPtr revIDLastSave="387" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{84A2480B-F1F3-4520-9285-6E792E3B27E0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56D738C3-148A-420A-8894-4D7B344C02BA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
   <si>
     <t>Fuente</t>
   </si>
@@ -271,6 +271,23 @@
   </si>
   <si>
     <t>15/5/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nuevas Disposiciones presidenciales en caso de calamidad pública 
+y órdenes para el estricto cumplimiento, 24 mayo 2020
+</t>
+  </si>
+  <si>
+    <t>25/5/2020</t>
+  </si>
+  <si>
+    <t>https://legal.dca.gob.gt/GestionDocumento/VisualizarDocumento?verDocumentoPrevia=True&amp;versionImpresa=False&amp;doc=60004</t>
+  </si>
+  <si>
+    <t>Acuerdo Gubernativo para la creación de la Comisión Presidencial de Atención a la Emergencia de Covid 19 ó Coprecovid</t>
+  </si>
+  <si>
+    <t>24/5/2020</t>
   </si>
 </sst>
 </file>
@@ -413,7 +430,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -479,6 +496,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -911,8 +937,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K12" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:K12" xr:uid="{EAF3A26F-8D4B-46F0-8F27-A70184B410C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K14" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:K14" xr:uid="{EAF3A26F-8D4B-46F0-8F27-A70184B410C1}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K11">
     <sortCondition descending="1" ref="I1:I11"/>
   </sortState>
@@ -1234,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355F3C84-FBC8-4F70-8922-1A1A2826C9C6}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -1647,12 +1673,74 @@
       </c>
       <c r="K12" s="21"/>
     </row>
-    <row r="13" spans="1:12" ht="15"/>
-    <row r="14" spans="1:12" ht="15"/>
+    <row r="13" spans="1:12" ht="60">
+      <c r="A13" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="16">
+        <f>+ROW()-1</f>
+        <v>12</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="19"/>
+      <c r="I13" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="21"/>
+    </row>
+    <row r="14" spans="1:12" ht="91.5" customHeight="1">
+      <c r="A14" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="16">
+        <f>+ROW()-1</f>
+        <v>13</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="19"/>
+      <c r="I14" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="21"/>
+    </row>
     <row r="15" spans="1:12" ht="15"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada no válida" error="Selecciona una categoría de la lista" promptTitle="Categoria" prompt="Selecciona una categoría de la lista" sqref="C2:C12" xr:uid="{6886B6D6-D01B-4A3E-AC32-C93F79577E67}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada no válida" error="Selecciona una categoría de la lista" promptTitle="Categoria" prompt="Selecciona una categoría de la lista" sqref="C2:C14" xr:uid="{6886B6D6-D01B-4A3E-AC32-C93F79577E67}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{2AEE38DF-B0A8-494B-AD95-04F5680089A1}"/>
@@ -1677,10 +1765,14 @@
     <hyperlink ref="E8" r:id="rId20" xr:uid="{0DDB8F11-8156-4600-BB4A-B8C956376579}"/>
     <hyperlink ref="E12" r:id="rId21" xr:uid="{9DCE4B16-82CC-4B45-B72F-C93FE98BEAFB}"/>
     <hyperlink ref="G12" r:id="rId22" xr:uid="{344E4542-DCF8-411A-926F-C6E068111423}"/>
+    <hyperlink ref="E13" r:id="rId23" xr:uid="{6434C0A2-AD70-4D5B-81B9-FF252B91D439}"/>
+    <hyperlink ref="G13" r:id="rId24" xr:uid="{25DE082D-C223-4EC6-B196-A119E8A3FCDA}"/>
+    <hyperlink ref="E14" r:id="rId25" xr:uid="{C7EFD1CD-EAC7-4503-95BE-C25EEC02D964}"/>
+    <hyperlink ref="G14" r:id="rId26" xr:uid="{303A5CD7-9DC1-4C36-A5DD-DD90EF1A73E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId23"/>
+    <tablePart r:id="rId27"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 06-05-2020 19-55-24
</commit_message>
<xml_diff>
--- a/datacovidgt/00 DATACOVID Trabajo_GT.xlsx
+++ b/datacovidgt/00 DATACOVID Trabajo_GT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22920"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23003"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID HN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="387" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{84A2480B-F1F3-4520-9285-6E792E3B27E0}"/>
+  <xr:revisionPtr revIDLastSave="397" documentId="13_ncr:1_{35734796-F087-4DAF-80FF-51295DFF148E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{85D9FEA4-3C51-4275-9B2F-5CE292510C18}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56D738C3-148A-420A-8894-4D7B344C02BA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="82">
   <si>
     <t>Fuente</t>
   </si>
@@ -288,6 +288,12 @@
   </si>
   <si>
     <t>24/5/2020</t>
+  </si>
+  <si>
+    <t>https://legal.dca.gob.gt/GestionDocumento/VisualizarDocumento?verDocumentoPrevia=True&amp;versionImpresa=False&amp;doc=60309</t>
+  </si>
+  <si>
+    <t>Estrategia Nacional de Control de Epidemia de SARS COV-2 y bases para la desescalada de los medios de reapertura condicionada del confinamiento</t>
   </si>
 </sst>
 </file>
@@ -430,7 +436,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -506,6 +512,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -937,8 +946,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K14" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
-  <autoFilter ref="A1:K14" xr:uid="{EAF3A26F-8D4B-46F0-8F27-A70184B410C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{412553A3-CE79-4C4C-963A-9E6A08424191}" name="Trabajo_CL" displayName="Trabajo_CL" ref="A1:K15" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:K15" xr:uid="{EAF3A26F-8D4B-46F0-8F27-A70184B410C1}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K11">
     <sortCondition descending="1" ref="I1:I11"/>
   </sortState>
@@ -1260,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355F3C84-FBC8-4F70-8922-1A1A2826C9C6}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -1737,10 +1746,41 @@
       </c>
       <c r="K14" s="21"/>
     </row>
-    <row r="15" spans="1:12" ht="15"/>
+    <row r="15" spans="1:12" ht="165">
+      <c r="A15" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="16">
+        <f>+ROW()-1</f>
+        <v>14</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="19"/>
+      <c r="I15" s="26">
+        <v>43896</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="21"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada no válida" error="Selecciona una categoría de la lista" promptTitle="Categoria" prompt="Selecciona una categoría de la lista" sqref="C2:C14" xr:uid="{6886B6D6-D01B-4A3E-AC32-C93F79577E67}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada no válida" error="Selecciona una categoría de la lista" promptTitle="Categoria" prompt="Selecciona una categoría de la lista" sqref="C2:C15" xr:uid="{6886B6D6-D01B-4A3E-AC32-C93F79577E67}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{2AEE38DF-B0A8-494B-AD95-04F5680089A1}"/>
@@ -1769,10 +1809,12 @@
     <hyperlink ref="G13" r:id="rId24" xr:uid="{25DE082D-C223-4EC6-B196-A119E8A3FCDA}"/>
     <hyperlink ref="E14" r:id="rId25" xr:uid="{C7EFD1CD-EAC7-4503-95BE-C25EEC02D964}"/>
     <hyperlink ref="G14" r:id="rId26" xr:uid="{303A5CD7-9DC1-4C36-A5DD-DD90EF1A73E8}"/>
+    <hyperlink ref="G15" r:id="rId27" xr:uid="{3445CF85-D4D5-4B5D-9759-FA7A2D7FFFE4}"/>
+    <hyperlink ref="E15" r:id="rId28" xr:uid="{541F0B1E-CB9C-4E49-838B-20DDC5F8B4BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId27"/>
+    <tablePart r:id="rId29"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>